<commit_message>
added preparer to sheets
</commit_message>
<xml_diff>
--- a/s2cDNASample/s2cDNASample_0648.xlsx
+++ b/s2cDNASample/s2cDNASample_0648.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/s2cDNASample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0235E6A-592B-2247-A344-3148CEB6F846}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF659F2-402B-1B4C-9A15-49158A6CCC93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="18920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24160" windowHeight="18920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>